<commit_message>
Accreditamento Hero correzzione file xlsx
S1#111DEDALUS0000
DEDALUS_SPA
HERO
5.2
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dedalusspa-my.sharepoint.com/personal/cristiano_sassi_dedalus_eu/Documents/Desktop/FSE2_VERBALE_PS/HERO_PS/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Devel\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\HERO\5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="378" documentId="8_{63E9DA7A-E562-4196-8B7D-ABAC9D8BE15A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8EC4E67D-22FE-4BFC-8735-1466F8ECD1C8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88144212-B2AD-48DD-88AA-68BDB4BFF3D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="23880" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="806" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="344">
   <si>
     <t>COME VALORIZZARE LA CHECKLIST (tab TestCases)</t>
   </si>
@@ -1331,6 +1331,12 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.e4ce19c234^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>sistemare le confiigurazione sul cliente per impostare correttamente il campo "purpose_of_use"</t>
+  </si>
+  <si>
+    <t>sistemare le confiigurazione sul cliente per impostare correttamente il campo "action_id"</t>
   </si>
 </sst>
 </file>
@@ -1752,6 +1758,18 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1773,18 +1791,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1861,10 +1867,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4249,10 +4251,10 @@
   <dimension ref="A1:T659"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B45" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="E59" sqref="E59"/>
+      <selection pane="bottomRight" activeCell="J42" sqref="J42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4298,12 +4300,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="35" t="s">
+      <c r="A2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="36"/>
-      <c r="C2" s="37"/>
-      <c r="D2" s="36"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="40"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4321,14 +4323,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="38" t="s">
+      <c r="A3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="39"/>
-      <c r="C3" s="44" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="36"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4346,12 +4348,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="40"/>
-      <c r="B4" s="41"/>
-      <c r="C4" s="44" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="36"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4370,12 +4372,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="42"/>
-      <c r="B5" s="43"/>
-      <c r="C5" s="44" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="36"/>
+      <c r="D5" s="40"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4393,8 +4395,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="33"/>
-      <c r="B6" s="34"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4527,16 +4529,16 @@
       <c r="E10" s="22" t="s">
         <v>56</v>
       </c>
-      <c r="F10" s="45">
+      <c r="F10" s="33">
         <v>45008</v>
       </c>
-      <c r="G10" s="46" t="s">
+      <c r="G10" s="34" t="s">
         <v>221</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="34" t="s">
         <v>219</v>
       </c>
-      <c r="I10" s="46" t="s">
+      <c r="I10" s="34" t="s">
         <v>220</v>
       </c>
       <c r="J10" s="25" t="s">
@@ -4571,7 +4573,7 @@
       <c r="E11" s="22" t="s">
         <v>58</v>
       </c>
-      <c r="F11" s="45">
+      <c r="F11" s="33">
         <v>45008</v>
       </c>
       <c r="G11" s="24" t="s">
@@ -4615,7 +4617,7 @@
       <c r="E12" s="22" t="s">
         <v>60</v>
       </c>
-      <c r="F12" s="45">
+      <c r="F12" s="33">
         <v>45008</v>
       </c>
       <c r="G12" s="24" t="s">
@@ -4659,7 +4661,7 @@
       <c r="E13" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F13" s="45">
+      <c r="F13" s="33">
         <v>45008</v>
       </c>
       <c r="G13" s="24" t="s">
@@ -4703,7 +4705,7 @@
       <c r="E14" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F14" s="45">
+      <c r="F14" s="33">
         <v>45008</v>
       </c>
       <c r="G14" s="24" t="s">
@@ -4731,7 +4733,9 @@
       <c r="O14" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="P14" s="25"/>
+      <c r="P14" s="25" t="s">
+        <v>342</v>
+      </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
       <c r="S14" s="27"/>
@@ -4755,7 +4759,7 @@
       <c r="E15" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F15" s="45">
+      <c r="F15" s="33">
         <v>45008</v>
       </c>
       <c r="G15" s="24" t="s">
@@ -4783,7 +4787,9 @@
       <c r="O15" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="P15" s="25"/>
+      <c r="P15" s="25" t="s">
+        <v>343</v>
+      </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
       <c r="S15" s="27"/>
@@ -4925,7 +4931,7 @@
       <c r="E19" s="22" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="45">
+      <c r="F19" s="33">
         <v>45008</v>
       </c>
       <c r="G19" s="24" t="s">
@@ -4979,7 +4985,7 @@
       <c r="E20" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F20" s="45">
+      <c r="F20" s="33">
         <v>45008</v>
       </c>
       <c r="G20" s="24" t="s">
@@ -5033,7 +5039,7 @@
       <c r="E21" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F21" s="45">
+      <c r="F21" s="33">
         <v>45008</v>
       </c>
       <c r="G21" s="24" t="s">
@@ -5127,10 +5133,10 @@
       <c r="E23" s="22" t="s">
         <v>83</v>
       </c>
-      <c r="F23" s="45">
+      <c r="F23" s="33">
         <v>45008</v>
       </c>
-      <c r="G23" s="45" t="s">
+      <c r="G23" s="33" t="s">
         <v>245</v>
       </c>
       <c r="H23" s="24" t="s">
@@ -5181,7 +5187,7 @@
       <c r="E24" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F24" s="45"/>
+      <c r="F24" s="33"/>
       <c r="G24" s="24"/>
       <c r="H24" s="24"/>
       <c r="I24" s="24"/>
@@ -5221,13 +5227,13 @@
       <c r="E25" s="22" t="s">
         <v>87</v>
       </c>
-      <c r="F25" s="45">
+      <c r="F25" s="33">
         <v>45008</v>
       </c>
       <c r="G25" s="24" t="s">
         <v>248</v>
       </c>
-      <c r="H25" s="47" t="s">
+      <c r="H25" s="35" t="s">
         <v>249</v>
       </c>
       <c r="I25" s="24" t="s">
@@ -5275,7 +5281,7 @@
       <c r="E26" s="22" t="s">
         <v>89</v>
       </c>
-      <c r="F26" s="45">
+      <c r="F26" s="33">
         <v>45008</v>
       </c>
       <c r="G26" s="24" t="s">
@@ -5329,7 +5335,7 @@
       <c r="E27" s="22" t="s">
         <v>91</v>
       </c>
-      <c r="F27" s="45">
+      <c r="F27" s="33">
         <v>45008</v>
       </c>
       <c r="G27" s="24" t="s">
@@ -5383,7 +5389,7 @@
       <c r="E28" s="22" t="s">
         <v>93</v>
       </c>
-      <c r="F28" s="45">
+      <c r="F28" s="33">
         <v>45008</v>
       </c>
       <c r="G28" s="24" t="s">
@@ -5437,7 +5443,7 @@
       <c r="E29" s="22" t="s">
         <v>95</v>
       </c>
-      <c r="F29" s="45">
+      <c r="F29" s="33">
         <v>45008</v>
       </c>
       <c r="G29" s="24" t="s">
@@ -5491,7 +5497,7 @@
       <c r="E30" s="22" t="s">
         <v>97</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F30" s="33">
         <v>45008</v>
       </c>
       <c r="G30" s="24" t="s">
@@ -5545,7 +5551,7 @@
       <c r="E31" s="22" t="s">
         <v>99</v>
       </c>
-      <c r="F31" s="45">
+      <c r="F31" s="33">
         <v>45008</v>
       </c>
       <c r="G31" s="24" t="s">
@@ -5599,7 +5605,7 @@
       <c r="E32" s="22" t="s">
         <v>101</v>
       </c>
-      <c r="F32" s="45">
+      <c r="F32" s="33">
         <v>45008</v>
       </c>
       <c r="G32" s="24" t="s">
@@ -5653,7 +5659,7 @@
       <c r="E33" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="F33" s="45">
+      <c r="F33" s="33">
         <v>45008</v>
       </c>
       <c r="G33" s="24" t="s">
@@ -5707,7 +5713,7 @@
       <c r="E34" s="22" t="s">
         <v>105</v>
       </c>
-      <c r="F34" s="45">
+      <c r="F34" s="33">
         <v>45008</v>
       </c>
       <c r="G34" s="24" t="s">
@@ -5761,7 +5767,7 @@
       <c r="E35" s="22" t="s">
         <v>107</v>
       </c>
-      <c r="F35" s="45">
+      <c r="F35" s="33">
         <v>45008</v>
       </c>
       <c r="G35" s="24" t="s">
@@ -5815,7 +5821,7 @@
       <c r="E36" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="F36" s="45">
+      <c r="F36" s="33">
         <v>45008</v>
       </c>
       <c r="G36" s="24" t="s">
@@ -5869,7 +5875,7 @@
       <c r="E37" s="22" t="s">
         <v>111</v>
       </c>
-      <c r="F37" s="45">
+      <c r="F37" s="33">
         <v>45008</v>
       </c>
       <c r="G37" s="24" t="s">
@@ -5923,7 +5929,7 @@
       <c r="E38" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="F38" s="45">
+      <c r="F38" s="33">
         <v>45008</v>
       </c>
       <c r="G38" s="24" t="s">
@@ -5977,7 +5983,7 @@
       <c r="E39" s="22" t="s">
         <v>115</v>
       </c>
-      <c r="F39" s="45">
+      <c r="F39" s="33">
         <v>45008</v>
       </c>
       <c r="G39" s="24" t="s">
@@ -6031,7 +6037,7 @@
       <c r="E40" s="22" t="s">
         <v>117</v>
       </c>
-      <c r="F40" s="45">
+      <c r="F40" s="33">
         <v>45008</v>
       </c>
       <c r="G40" s="24" t="s">
@@ -6085,7 +6091,7 @@
       <c r="E41" s="22" t="s">
         <v>119</v>
       </c>
-      <c r="F41" s="45">
+      <c r="F41" s="33">
         <v>45008</v>
       </c>
       <c r="G41" s="24" t="s">
@@ -6139,7 +6145,7 @@
       <c r="E42" s="22" t="s">
         <v>177</v>
       </c>
-      <c r="F42" s="45">
+      <c r="F42" s="33">
         <v>45008</v>
       </c>
       <c r="G42" s="24" t="s">
@@ -6150,6 +6156,9 @@
       </c>
       <c r="I42" s="24" t="s">
         <v>301</v>
+      </c>
+      <c r="J42" s="25" t="s">
+        <v>68</v>
       </c>
       <c r="P42" s="25"/>
       <c r="Q42" s="25"/>
@@ -6175,7 +6184,7 @@
       <c r="E43" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="F43" s="45">
+      <c r="F43" s="33">
         <v>45008</v>
       </c>
       <c r="G43" s="24" t="s">
@@ -6187,7 +6196,9 @@
       <c r="I43" s="24" t="s">
         <v>304</v>
       </c>
-      <c r="J43" s="25"/>
+      <c r="J43" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="K43" s="25"/>
       <c r="L43" s="25"/>
       <c r="M43" s="25"/>
@@ -6217,7 +6228,7 @@
       <c r="E44" s="22" t="s">
         <v>181</v>
       </c>
-      <c r="F44" s="45">
+      <c r="F44" s="33">
         <v>45008</v>
       </c>
       <c r="G44" s="24" t="s">
@@ -6229,7 +6240,9 @@
       <c r="I44" s="24" t="s">
         <v>307</v>
       </c>
-      <c r="J44" s="25"/>
+      <c r="J44" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="K44" s="25"/>
       <c r="L44" s="25"/>
       <c r="M44" s="25"/>
@@ -6259,7 +6272,7 @@
       <c r="E45" s="22" t="s">
         <v>183</v>
       </c>
-      <c r="F45" s="45">
+      <c r="F45" s="33">
         <v>45008</v>
       </c>
       <c r="G45" s="24" t="s">
@@ -6271,7 +6284,9 @@
       <c r="I45" s="24" t="s">
         <v>310</v>
       </c>
-      <c r="J45" s="25"/>
+      <c r="J45" s="25" t="s">
+        <v>68</v>
+      </c>
       <c r="K45" s="25"/>
       <c r="L45" s="25"/>
       <c r="M45" s="25"/>
@@ -6301,7 +6316,7 @@
       <c r="E46" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="F46" s="45">
+      <c r="F46" s="33">
         <v>45008</v>
       </c>
       <c r="G46" s="24" t="s">
@@ -6329,7 +6344,9 @@
       <c r="O46" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="P46" s="25"/>
+      <c r="P46" s="25" t="s">
+        <v>342</v>
+      </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
       <c r="S46" s="27"/>
@@ -6353,7 +6370,7 @@
       <c r="E47" s="22" t="s">
         <v>66</v>
       </c>
-      <c r="F47" s="45">
+      <c r="F47" s="33">
         <v>45008</v>
       </c>
       <c r="G47" s="24" t="s">
@@ -6381,7 +6398,9 @@
       <c r="O47" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="P47" s="25"/>
+      <c r="P47" s="25" t="s">
+        <v>343</v>
+      </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
       <c r="S47" s="27"/>
@@ -6443,7 +6462,7 @@
       <c r="E49" s="22" t="s">
         <v>188</v>
       </c>
-      <c r="F49" s="45"/>
+      <c r="F49" s="33"/>
       <c r="G49" s="24"/>
       <c r="H49" s="24"/>
       <c r="I49" s="24"/>
@@ -6523,10 +6542,10 @@
       <c r="E51" s="22" t="s">
         <v>192</v>
       </c>
-      <c r="F51" s="45">
+      <c r="F51" s="33">
         <v>45008</v>
       </c>
-      <c r="G51" s="48" t="s">
+      <c r="G51" s="36" t="s">
         <v>316</v>
       </c>
       <c r="H51" s="24" t="s">
@@ -6577,7 +6596,7 @@
       <c r="E52" s="22" t="s">
         <v>194</v>
       </c>
-      <c r="F52" s="45">
+      <c r="F52" s="33">
         <v>45008</v>
       </c>
       <c r="G52" s="24" t="s">
@@ -6631,7 +6650,7 @@
       <c r="E53" s="22" t="s">
         <v>196</v>
       </c>
-      <c r="F53" s="45">
+      <c r="F53" s="33">
         <v>45008</v>
       </c>
       <c r="G53" s="24" t="s">
@@ -6724,7 +6743,7 @@
       <c r="E55" s="22" t="s">
         <v>200</v>
       </c>
-      <c r="F55" s="45">
+      <c r="F55" s="33">
         <v>45008</v>
       </c>
       <c r="G55" s="24" t="s">
@@ -6778,10 +6797,10 @@
       <c r="E56" s="22" t="s">
         <v>202</v>
       </c>
-      <c r="F56" s="45">
+      <c r="F56" s="33">
         <v>45008</v>
       </c>
-      <c r="G56" s="48" t="s">
+      <c r="G56" s="36" t="s">
         <v>327</v>
       </c>
       <c r="H56" s="24" t="s">
@@ -6832,7 +6851,7 @@
       <c r="E57" s="22" t="s">
         <v>204</v>
       </c>
-      <c r="F57" s="45">
+      <c r="F57" s="33">
         <v>45008</v>
       </c>
       <c r="G57" s="24" t="s">
@@ -6886,7 +6905,7 @@
       <c r="E58" s="22" t="s">
         <v>206</v>
       </c>
-      <c r="F58" s="45">
+      <c r="F58" s="33">
         <v>45008</v>
       </c>
       <c r="G58" s="24" t="s">
@@ -6940,7 +6959,7 @@
       <c r="E59" s="22" t="s">
         <v>208</v>
       </c>
-      <c r="F59" s="45">
+      <c r="F59" s="33">
         <v>45008</v>
       </c>
       <c r="G59" s="24" t="s">
@@ -6994,7 +7013,7 @@
       <c r="E60" s="22" t="s">
         <v>210</v>
       </c>
-      <c r="F60" s="45">
+      <c r="F60" s="33">
         <v>45008</v>
       </c>
       <c r="G60" s="24" t="s">
@@ -16330,7 +16349,7 @@
           <x14:formula1>
             <xm:f>Sheet1!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>O46:O47 J46:J47 L46:M47 L49:M60 L10:M41 J49:J60 J10:J41 O49:O60 O10:O41</xm:sqref>
+          <xm:sqref>O46:O47 L46:M47 L49:M60 L10:M41 J49:J60 O49:O60 O10:O41 J10:J47</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0200-000001000000}">
           <x14:formula1>

</xml_diff>

<commit_message>
sistemate segnalazioni 18 aprile
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Devel\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\HERO\5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD5E3A52-0D10-422F-9E32-0EB4A5A1B8DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBAEC0-2CF5-4EDC-A9D6-75E2537AB34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1050" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1050" yWindow="-120" windowWidth="23070" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Istruzioni Compilazione" sheetId="1" r:id="rId1"/>
@@ -964,57 +964,9 @@
     <t>Il campo deve essere sempre  compilato dall'operatore</t>
   </si>
   <si>
-    <t>cf7e69e8b08bd663</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.e1689675671bf44d272c6ee39d2acc7bbdeb7860fac3868ff0b2368dd832b87d.3e41e96d9a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T09:16:00Z</t>
-  </si>
-  <si>
-    <t>2023-03-23T09:20:36Z</t>
-  </si>
-  <si>
-    <t>f2ac9471b2655e7e</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.1181c3abf43e3db497ed6138062b3587ee0461464cf24afdc304c7387eeb8a03.d90a4975e6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T09:22:39Z</t>
-  </si>
-  <si>
-    <t>23c06e72e4171d02</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.4c083e2fd0252d4d741c1d91e37f7a08faaba81283a736d5d4c1062614b5c67d.41b806335c^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T09:24:09Z</t>
-  </si>
-  <si>
-    <t>c11f8aa018c01231</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.c4e3b0df69c3aa128a9f26f4a492453e199b680dff77957040ee12927f49cd33.53f071c0e7^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T09:30:25Z</t>
-  </si>
-  <si>
-    <t>09327b559d62d2aa</t>
-  </si>
-  <si>
     <t>UNKNOWN_WORKFLOW_ID</t>
   </si>
   <si>
-    <t>6f43622f79ddae48</t>
-  </si>
-  <si>
-    <t>2023-02-23T09:35:58Z</t>
-  </si>
-  <si>
     <t>7cedd330ffc8ac89</t>
   </si>
   <si>
@@ -1202,54 +1154,6 @@
   </si>
   <si>
     <t>2.16.840.1.113883.2.9.2.150.4.4.c4e3b0df69c3aa128a9f26f4a492453e199b680dff77957040ee12927f49cd33.85f3b5eaa6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T13:15:48Z</t>
-  </si>
-  <si>
-    <t>9866ca75198425de</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.b09a5bf06f3376484421947a7583f649c8267ceaae72a3b470caf6f8163995b2.f494d1ddbd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T13:16:51Z</t>
-  </si>
-  <si>
-    <t>684cfd3aa6ac5d66</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.fba3831dcd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T13:21:34Z</t>
-  </si>
-  <si>
-    <t>b2729c1fcd3a1739</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.7c575e0e4a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T13:24:37Z</t>
-  </si>
-  <si>
-    <t>927c63b61e5560bc</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.0f3067ff47^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-03-23T13:26:06Z</t>
-  </si>
-  <si>
-    <t>873cb9fcd9006e75</t>
-  </si>
-  <si>
-    <t>2023-03-23T13:28:05Z</t>
-  </si>
-  <si>
-    <t>6ce4c035659ba0b3</t>
   </si>
   <si>
     <t>95a605908da7ee80</t>
@@ -1542,42 +1446,6 @@
     <t>18702999f3841d1a</t>
   </si>
   <si>
-    <t>2023-04-06T17:11:36Z</t>
-  </si>
-  <si>
-    <t>bbca5bb566c601e1</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.0bada2628a915e683ae1850e263ec2587a0d5d1042803419829fc922dec26c5b.ff7a3960b0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-06T17:14:32Z</t>
-  </si>
-  <si>
-    <t>142f8ea1113d14a6</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.9d2810e4b8d89b76fcd3d3a20fb907bf12b4359d15910985725131df945e509b.ed73671ad8^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-06T17:17:57Z</t>
-  </si>
-  <si>
-    <t>24dce9581f1b872d</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.330734ed8ddfaee1745e7cbb033f2e0ae3001fbbc75497e5e4efb1f797aa19dc.b04bef7ba2^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-06T17:19:59Z</t>
-  </si>
-  <si>
-    <t>6e93ca2d98e5139f</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.934167a59c9f6667655d91d04807f0b8b2283f57358e23960660542ea9ba4327.c37238560f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>2023-04-06T17:23:18Z</t>
   </si>
   <si>
@@ -1708,6 +1576,138 @@
   </si>
   <si>
     <t>Il campo è sempre impostato a 'S' visto che è prevista solo la gestione di documenti firmati digitalmente</t>
+  </si>
+  <si>
+    <t>2023-04-18T14:35:32Z</t>
+  </si>
+  <si>
+    <t>c9e822bcec522eff</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.e1689675671bf44d272c6ee39d2acc7bbdeb7860fac3868ff0b2368dd832b87d.9687299faa^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T14:50:39Z</t>
+  </si>
+  <si>
+    <t>bb63d585c5d570c7</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.1181c3abf43e3db497ed6138062b3587ee0461464cf24afdc304c7387eeb8a03.8a310d0e20^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T14:59:51Z</t>
+  </si>
+  <si>
+    <t>5f3213c8021280b3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.4c083e2fd0252d4d741c1d91e37f7a08faaba81283a736d5d4c1062614b5c67d.59bfc4ecb6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:14:57Z</t>
+  </si>
+  <si>
+    <t>47d1566689772b77</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.c4e3b0df69c3aa128a9f26f4a492453e199b680dff77957040ee12927f49cd33.99499b9e77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>3e41c3314382acb7</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:19:11Z</t>
+  </si>
+  <si>
+    <t>6c2a84e9adbd0c64</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:21:47Z</t>
+  </si>
+  <si>
+    <t>eda5f3a8f4364f5f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.b09a5bf06f3376484421947a7583f649c8267ceaae72a3b470caf6f8163995b2.4270c059cd^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:28:35Z</t>
+  </si>
+  <si>
+    <t>e1cd64b83889f6eb</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.cdfd820856^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>1197489d746bd724</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.4e919bf9ff^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:31:26Z</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:30:18Z</t>
+  </si>
+  <si>
+    <t>89549341478787b4</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:35:05Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.51d8dd163bda384bb646392e73b7089b70ddcb0efa596412a6e4aaf00633fff8.bd44cf997a^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>5eaebea68d47ecc3</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:36:12Z</t>
+  </si>
+  <si>
+    <t>0f6324059b71374a</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:40:46Z</t>
+  </si>
+  <si>
+    <t>2023-04-18T15:47:25Z</t>
+  </si>
+  <si>
+    <t>63c8607fd053988f</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.0bada2628a915e683ae1850e263ec2587a0d5d1042803419829fc922dec26c5b.5244963f69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>f79823d2fc5ea9d3</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.9d2810e4b8d89b76fcd3d3a20fb907bf12b4359d15910985725131df945e509b.39c0b575bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T16:03:53Z</t>
+  </si>
+  <si>
+    <t>eddc22525d89a0b5</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.330734ed8ddfaee1745e7cbb033f2e0ae3001fbbc75497e5e4efb1f797aa19dc.edafa62317^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-18T16:41:32Z</t>
+  </si>
+  <si>
+    <t>e590df00ddc4a306</t>
+  </si>
+  <si>
+    <t>2023-04-18T16:43:17Z</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.934167a59c9f6667655d91d04807f0b8b2283f57358e23960660542ea9ba4327.9f7f91b5f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
 </sst>
 </file>
@@ -2039,7 +2039,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="50">
+  <cellXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -2165,6 +2165,15 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4624,23 +4633,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:T659"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="D82" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="1" ySplit="6" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G85" sqref="G85"/>
+      <selection pane="bottomRight" activeCell="G67" sqref="G67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="15.42578125" customWidth="1"/>
+    <col min="1" max="1" width="11.42578125" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="8.140625" customWidth="1"/>
-    <col min="4" max="4" width="48.85546875" customWidth="1"/>
-    <col min="5" max="5" width="58.5703125" customWidth="1"/>
+    <col min="4" max="4" width="31.28515625" customWidth="1"/>
+    <col min="5" max="5" width="49" customWidth="1"/>
     <col min="6" max="6" width="25" customWidth="1"/>
     <col min="7" max="7" width="27.42578125" customWidth="1"/>
-    <col min="8" max="8" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" customWidth="1"/>
     <col min="9" max="9" width="57" customWidth="1"/>
     <col min="10" max="10" width="16.7109375" customWidth="1"/>
     <col min="11" max="11" width="12.5703125" customWidth="1"/>
@@ -4904,16 +4913,16 @@
         <v>56</v>
       </c>
       <c r="F10" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G10" s="34" t="s">
-        <v>221</v>
-      </c>
-      <c r="H10" s="34" t="s">
-        <v>219</v>
+        <v>45034</v>
+      </c>
+      <c r="G10" s="51" t="s">
+        <v>408</v>
+      </c>
+      <c r="H10" s="50" t="s">
+        <v>409</v>
       </c>
       <c r="I10" s="34" t="s">
-        <v>220</v>
+        <v>410</v>
       </c>
       <c r="J10" s="25" t="s">
         <v>68</v>
@@ -4948,16 +4957,16 @@
         <v>58</v>
       </c>
       <c r="F11" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>222</v>
+        <v>45034</v>
+      </c>
+      <c r="G11" s="51" t="s">
+        <v>411</v>
       </c>
       <c r="H11" s="24" t="s">
-        <v>223</v>
-      </c>
-      <c r="I11" s="24" t="s">
-        <v>224</v>
+        <v>412</v>
+      </c>
+      <c r="I11" s="36" t="s">
+        <v>413</v>
       </c>
       <c r="J11" s="25" t="s">
         <v>68</v>
@@ -4992,16 +5001,16 @@
         <v>60</v>
       </c>
       <c r="F12" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>225</v>
+        <v>45034</v>
+      </c>
+      <c r="G12" s="51" t="s">
+        <v>414</v>
       </c>
       <c r="H12" s="24" t="s">
-        <v>226</v>
+        <v>415</v>
       </c>
       <c r="I12" s="24" t="s">
-        <v>227</v>
+        <v>416</v>
       </c>
       <c r="J12" s="25" t="s">
         <v>68</v>
@@ -5036,16 +5045,16 @@
         <v>62</v>
       </c>
       <c r="F13" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>228</v>
+        <v>45034</v>
+      </c>
+      <c r="G13" s="51" t="s">
+        <v>417</v>
       </c>
       <c r="H13" s="24" t="s">
-        <v>229</v>
+        <v>418</v>
       </c>
       <c r="I13" s="24" t="s">
-        <v>230</v>
+        <v>419</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>68</v>
@@ -5076,20 +5085,20 @@
       <c r="D14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="52" t="s">
         <v>64</v>
       </c>
       <c r="F14" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>231</v>
+        <v>45034</v>
+      </c>
+      <c r="G14" s="51" t="s">
+        <v>421</v>
       </c>
       <c r="H14" s="24" t="s">
-        <v>232</v>
+        <v>420</v>
       </c>
       <c r="I14" s="24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J14" s="25" t="s">
         <v>68</v>
@@ -5108,7 +5117,7 @@
         <v>172</v>
       </c>
       <c r="P14" s="25" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="Q14" s="25"/>
       <c r="R14" s="26"/>
@@ -5130,20 +5139,20 @@
       <c r="D15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="52" t="s">
         <v>66</v>
       </c>
       <c r="F15" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G15" s="24" t="s">
-        <v>235</v>
+        <v>45034</v>
+      </c>
+      <c r="G15" s="51" t="s">
+        <v>423</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>234</v>
+        <v>422</v>
       </c>
       <c r="I15" s="24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J15" s="25" t="s">
         <v>68</v>
@@ -5162,7 +5171,7 @@
         <v>172</v>
       </c>
       <c r="P15" s="25" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="Q15" s="25"/>
       <c r="R15" s="26"/>
@@ -5311,13 +5320,13 @@
         <v>45008</v>
       </c>
       <c r="G19" s="24" t="s">
-        <v>237</v>
+        <v>221</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>236</v>
+        <v>220</v>
       </c>
       <c r="I19" s="24" t="s">
-        <v>238</v>
+        <v>222</v>
       </c>
       <c r="J19" s="25" t="s">
         <v>68</v>
@@ -5365,13 +5374,13 @@
         <v>45008</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>241</v>
+        <v>225</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>239</v>
+        <v>223</v>
       </c>
       <c r="I20" s="24" t="s">
-        <v>240</v>
+        <v>224</v>
       </c>
       <c r="J20" s="25" t="s">
         <v>68</v>
@@ -5419,13 +5428,13 @@
         <v>45008</v>
       </c>
       <c r="G21" s="24" t="s">
-        <v>243</v>
+        <v>227</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>242</v>
+        <v>226</v>
       </c>
       <c r="I21" s="24" t="s">
-        <v>244</v>
+        <v>228</v>
       </c>
       <c r="J21" s="25" t="s">
         <v>68</v>
@@ -5513,13 +5522,13 @@
         <v>45008</v>
       </c>
       <c r="G23" s="33" t="s">
-        <v>245</v>
+        <v>229</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>246</v>
+        <v>230</v>
       </c>
       <c r="I23" s="24" t="s">
-        <v>247</v>
+        <v>231</v>
       </c>
       <c r="J23" s="25" t="s">
         <v>68</v>
@@ -5607,13 +5616,13 @@
         <v>45008</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>248</v>
+        <v>232</v>
       </c>
       <c r="H25" s="35" t="s">
-        <v>249</v>
+        <v>233</v>
       </c>
       <c r="I25" s="24" t="s">
-        <v>250</v>
+        <v>234</v>
       </c>
       <c r="J25" s="25" t="s">
         <v>68</v>
@@ -5661,13 +5670,13 @@
         <v>45008</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>251</v>
+        <v>235</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>252</v>
+        <v>236</v>
       </c>
       <c r="I26" s="24" t="s">
-        <v>253</v>
+        <v>237</v>
       </c>
       <c r="J26" s="25" t="s">
         <v>68</v>
@@ -5715,13 +5724,13 @@
         <v>45008</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>254</v>
+        <v>238</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>255</v>
+        <v>239</v>
       </c>
       <c r="I27" s="24" t="s">
-        <v>256</v>
+        <v>240</v>
       </c>
       <c r="J27" s="25" t="s">
         <v>68</v>
@@ -5769,13 +5778,13 @@
         <v>45008</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>257</v>
+        <v>241</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>258</v>
+        <v>242</v>
       </c>
       <c r="I28" s="24" t="s">
-        <v>259</v>
+        <v>243</v>
       </c>
       <c r="J28" s="25" t="s">
         <v>68</v>
@@ -5823,13 +5832,13 @@
         <v>45008</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>261</v>
+        <v>245</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>260</v>
+        <v>244</v>
       </c>
       <c r="I29" s="24" t="s">
-        <v>262</v>
+        <v>246</v>
       </c>
       <c r="J29" s="25" t="s">
         <v>68</v>
@@ -5877,13 +5886,13 @@
         <v>45008</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>263</v>
+        <v>247</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>264</v>
+        <v>248</v>
       </c>
       <c r="I30" s="24" t="s">
-        <v>265</v>
+        <v>249</v>
       </c>
       <c r="J30" s="25" t="s">
         <v>68</v>
@@ -5931,13 +5940,13 @@
         <v>45008</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>267</v>
+        <v>251</v>
       </c>
       <c r="I31" s="24" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="J31" s="25" t="s">
         <v>68</v>
@@ -5985,13 +5994,13 @@
         <v>45008</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>271</v>
+        <v>255</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>269</v>
+        <v>253</v>
       </c>
       <c r="I32" s="24" t="s">
-        <v>270</v>
+        <v>254</v>
       </c>
       <c r="J32" s="25" t="s">
         <v>68</v>
@@ -6039,13 +6048,13 @@
         <v>45008</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>272</v>
+        <v>256</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>273</v>
+        <v>257</v>
       </c>
       <c r="I33" s="24" t="s">
-        <v>274</v>
+        <v>258</v>
       </c>
       <c r="J33" s="25" t="s">
         <v>68</v>
@@ -6093,13 +6102,13 @@
         <v>45008</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>275</v>
+        <v>259</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>276</v>
+        <v>260</v>
       </c>
       <c r="I34" s="24" t="s">
-        <v>277</v>
+        <v>261</v>
       </c>
       <c r="J34" s="25" t="s">
         <v>68</v>
@@ -6147,13 +6156,13 @@
         <v>45008</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>278</v>
+        <v>262</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>279</v>
+        <v>263</v>
       </c>
       <c r="I35" s="24" t="s">
-        <v>280</v>
+        <v>264</v>
       </c>
       <c r="J35" s="25" t="s">
         <v>68</v>
@@ -6201,13 +6210,13 @@
         <v>45008</v>
       </c>
       <c r="G36" s="24" t="s">
-        <v>282</v>
+        <v>266</v>
       </c>
       <c r="H36" s="24" t="s">
-        <v>281</v>
+        <v>265</v>
       </c>
       <c r="I36" s="24" t="s">
-        <v>283</v>
+        <v>267</v>
       </c>
       <c r="J36" s="25" t="s">
         <v>68</v>
@@ -6255,13 +6264,13 @@
         <v>45008</v>
       </c>
       <c r="G37" s="24" t="s">
-        <v>284</v>
+        <v>268</v>
       </c>
       <c r="H37" s="24" t="s">
-        <v>285</v>
+        <v>269</v>
       </c>
       <c r="I37" s="24" t="s">
-        <v>286</v>
+        <v>270</v>
       </c>
       <c r="J37" s="25" t="s">
         <v>68</v>
@@ -6309,13 +6318,13 @@
         <v>45008</v>
       </c>
       <c r="G38" s="24" t="s">
-        <v>288</v>
+        <v>272</v>
       </c>
       <c r="H38" s="24" t="s">
-        <v>287</v>
+        <v>271</v>
       </c>
       <c r="I38" s="24" t="s">
-        <v>289</v>
+        <v>273</v>
       </c>
       <c r="J38" s="25" t="s">
         <v>68</v>
@@ -6363,13 +6372,13 @@
         <v>45008</v>
       </c>
       <c r="G39" s="24" t="s">
-        <v>290</v>
+        <v>274</v>
       </c>
       <c r="H39" s="24" t="s">
-        <v>291</v>
+        <v>275</v>
       </c>
       <c r="I39" s="24" t="s">
-        <v>292</v>
+        <v>276</v>
       </c>
       <c r="J39" s="25" t="s">
         <v>68</v>
@@ -6417,13 +6426,13 @@
         <v>45008</v>
       </c>
       <c r="G40" s="24" t="s">
-        <v>293</v>
+        <v>277</v>
       </c>
       <c r="H40" s="24" t="s">
-        <v>294</v>
+        <v>278</v>
       </c>
       <c r="I40" s="24" t="s">
-        <v>295</v>
+        <v>279</v>
       </c>
       <c r="J40" s="25" t="s">
         <v>68</v>
@@ -6451,7 +6460,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="41" spans="1:20" ht="195.75" thickBot="1">
+    <row r="41" spans="1:20" ht="225.75" thickBot="1">
       <c r="A41" s="20">
         <v>146</v>
       </c>
@@ -6471,13 +6480,13 @@
         <v>45008</v>
       </c>
       <c r="G41" s="24" t="s">
-        <v>296</v>
+        <v>280</v>
       </c>
       <c r="H41" s="24" t="s">
-        <v>297</v>
+        <v>281</v>
       </c>
       <c r="I41" s="24" t="s">
-        <v>298</v>
+        <v>282</v>
       </c>
       <c r="J41" s="25" t="s">
         <v>68</v>
@@ -6505,7 +6514,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="42" spans="1:20" ht="225.75" thickBot="1">
+    <row r="42" spans="1:20" ht="270.75" thickBot="1">
       <c r="A42" s="20">
         <v>6</v>
       </c>
@@ -6522,16 +6531,16 @@
         <v>177</v>
       </c>
       <c r="F42" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G42" s="24" t="s">
-        <v>299</v>
+        <v>45034</v>
+      </c>
+      <c r="G42" s="51" t="s">
+        <v>426</v>
       </c>
       <c r="H42" s="24" t="s">
-        <v>300</v>
-      </c>
-      <c r="I42" s="24" t="s">
-        <v>301</v>
+        <v>424</v>
+      </c>
+      <c r="I42" s="36" t="s">
+        <v>425</v>
       </c>
       <c r="J42" s="37" t="s">
         <v>68</v>
@@ -6544,7 +6553,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" spans="1:20" ht="225.75" thickBot="1">
+    <row r="43" spans="1:20" ht="270.75" thickBot="1">
       <c r="A43" s="20">
         <v>7</v>
       </c>
@@ -6561,16 +6570,16 @@
         <v>179</v>
       </c>
       <c r="F43" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G43" s="24" t="s">
-        <v>302</v>
+        <v>45034</v>
+      </c>
+      <c r="G43" s="36" t="s">
+        <v>432</v>
       </c>
       <c r="H43" s="24" t="s">
-        <v>303</v>
-      </c>
-      <c r="I43" s="24" t="s">
-        <v>304</v>
+        <v>427</v>
+      </c>
+      <c r="I43" s="36" t="s">
+        <v>428</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>68</v>
@@ -6588,7 +6597,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="44" spans="1:20" ht="225.75" thickBot="1">
+    <row r="44" spans="1:20" ht="270.75" thickBot="1">
       <c r="A44" s="20">
         <v>8</v>
       </c>
@@ -6605,16 +6614,16 @@
         <v>181</v>
       </c>
       <c r="F44" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G44" s="24" t="s">
-        <v>305</v>
+        <v>45034</v>
+      </c>
+      <c r="G44" s="36" t="s">
+        <v>431</v>
       </c>
       <c r="H44" s="24" t="s">
-        <v>306</v>
-      </c>
-      <c r="I44" s="24" t="s">
-        <v>307</v>
+        <v>429</v>
+      </c>
+      <c r="I44" s="36" t="s">
+        <v>430</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>68</v>
@@ -6632,7 +6641,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="45" spans="1:20" ht="225.75" thickBot="1">
+    <row r="45" spans="1:20" ht="270.75" thickBot="1">
       <c r="A45" s="20">
         <v>9</v>
       </c>
@@ -6649,16 +6658,16 @@
         <v>183</v>
       </c>
       <c r="F45" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>308</v>
-      </c>
-      <c r="H45" s="24" t="s">
-        <v>309</v>
+        <v>45034</v>
+      </c>
+      <c r="G45" s="36" t="s">
+        <v>434</v>
+      </c>
+      <c r="H45" s="35" t="s">
+        <v>433</v>
       </c>
       <c r="I45" s="24" t="s">
-        <v>310</v>
+        <v>435</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>68</v>
@@ -6676,7 +6685,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="46" spans="1:20" ht="225.75" thickBot="1">
+    <row r="46" spans="1:20" ht="240.75" thickBot="1">
       <c r="A46" s="20">
         <v>29</v>
       </c>
@@ -6693,16 +6702,16 @@
         <v>64</v>
       </c>
       <c r="F46" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G46" s="24" t="s">
-        <v>311</v>
+        <v>45034</v>
+      </c>
+      <c r="G46" s="36" t="s">
+        <v>437</v>
       </c>
       <c r="H46" s="24" t="s">
-        <v>312</v>
+        <v>436</v>
       </c>
       <c r="I46" s="24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J46" s="25" t="s">
         <v>68</v>
@@ -6721,7 +6730,7 @@
         <v>172</v>
       </c>
       <c r="P46" s="25" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="Q46" s="25"/>
       <c r="R46" s="26"/>
@@ -6730,7 +6739,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="47" spans="1:20" ht="210.75" thickBot="1">
+    <row r="47" spans="1:20" ht="255.75" thickBot="1">
       <c r="A47" s="20">
         <v>37</v>
       </c>
@@ -6743,20 +6752,20 @@
       <c r="D47" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E47" s="52" t="s">
         <v>66</v>
       </c>
       <c r="F47" s="33">
-        <v>45008</v>
-      </c>
-      <c r="G47" s="24" t="s">
-        <v>313</v>
+        <v>45034</v>
+      </c>
+      <c r="G47" s="36" t="s">
+        <v>439</v>
       </c>
       <c r="H47" s="24" t="s">
-        <v>314</v>
+        <v>438</v>
       </c>
       <c r="I47" s="24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J47" s="25" t="s">
         <v>68</v>
@@ -6775,7 +6784,7 @@
         <v>172</v>
       </c>
       <c r="P47" s="25" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="Q47" s="25"/>
       <c r="R47" s="26"/>
@@ -6924,13 +6933,13 @@
         <v>45008</v>
       </c>
       <c r="G51" s="36" t="s">
-        <v>316</v>
+        <v>284</v>
       </c>
       <c r="H51" s="24" t="s">
-        <v>315</v>
+        <v>283</v>
       </c>
       <c r="I51" s="24" t="s">
-        <v>317</v>
+        <v>285</v>
       </c>
       <c r="J51" s="25" t="s">
         <v>68</v>
@@ -6978,13 +6987,13 @@
         <v>45008</v>
       </c>
       <c r="G52" s="24" t="s">
-        <v>318</v>
+        <v>286</v>
       </c>
       <c r="H52" s="24" t="s">
-        <v>319</v>
+        <v>287</v>
       </c>
       <c r="I52" s="24" t="s">
-        <v>320</v>
+        <v>288</v>
       </c>
       <c r="J52" s="25" t="s">
         <v>68</v>
@@ -7032,13 +7041,13 @@
         <v>45008</v>
       </c>
       <c r="G53" s="24" t="s">
-        <v>322</v>
+        <v>290</v>
       </c>
       <c r="H53" s="24" t="s">
-        <v>321</v>
+        <v>289</v>
       </c>
       <c r="I53" s="24" t="s">
-        <v>323</v>
+        <v>291</v>
       </c>
       <c r="J53" s="25" t="s">
         <v>68</v>
@@ -7125,13 +7134,13 @@
         <v>45008</v>
       </c>
       <c r="G55" s="24" t="s">
-        <v>325</v>
+        <v>293</v>
       </c>
       <c r="H55" s="24" t="s">
-        <v>324</v>
+        <v>292</v>
       </c>
       <c r="I55" s="24" t="s">
-        <v>326</v>
+        <v>294</v>
       </c>
       <c r="J55" s="25" t="s">
         <v>68</v>
@@ -7179,13 +7188,13 @@
         <v>45008</v>
       </c>
       <c r="G56" s="36" t="s">
-        <v>327</v>
+        <v>295</v>
       </c>
       <c r="H56" s="24" t="s">
-        <v>328</v>
+        <v>296</v>
       </c>
       <c r="I56" s="24" t="s">
-        <v>329</v>
+        <v>297</v>
       </c>
       <c r="J56" s="25" t="s">
         <v>68</v>
@@ -7233,13 +7242,13 @@
         <v>45008</v>
       </c>
       <c r="G57" s="24" t="s">
-        <v>330</v>
+        <v>298</v>
       </c>
       <c r="H57" s="24" t="s">
-        <v>331</v>
+        <v>299</v>
       </c>
       <c r="I57" s="24" t="s">
-        <v>332</v>
+        <v>300</v>
       </c>
       <c r="J57" s="25" t="s">
         <v>68</v>
@@ -7287,13 +7296,13 @@
         <v>45008</v>
       </c>
       <c r="G58" s="24" t="s">
-        <v>333</v>
+        <v>301</v>
       </c>
       <c r="H58" s="24" t="s">
-        <v>334</v>
+        <v>302</v>
       </c>
       <c r="I58" s="24" t="s">
-        <v>335</v>
+        <v>303</v>
       </c>
       <c r="J58" s="25" t="s">
         <v>68</v>
@@ -7341,13 +7350,13 @@
         <v>45008</v>
       </c>
       <c r="G59" s="24" t="s">
-        <v>336</v>
+        <v>304</v>
       </c>
       <c r="H59" s="24" t="s">
-        <v>337</v>
+        <v>305</v>
       </c>
       <c r="I59" s="24" t="s">
-        <v>338</v>
+        <v>306</v>
       </c>
       <c r="J59" s="25" t="s">
         <v>68</v>
@@ -7395,13 +7404,13 @@
         <v>45008</v>
       </c>
       <c r="G60" s="24" t="s">
-        <v>339</v>
+        <v>307</v>
       </c>
       <c r="H60" s="24" t="s">
-        <v>340</v>
+        <v>308</v>
       </c>
       <c r="I60" s="24" t="s">
-        <v>341</v>
+        <v>309</v>
       </c>
       <c r="J60" s="25" t="s">
         <v>68</v>
@@ -7440,7 +7449,7 @@
         <v>52</v>
       </c>
       <c r="D61" s="21" t="s">
-        <v>343</v>
+        <v>311</v>
       </c>
       <c r="E61" s="22" t="s">
         <v>64</v>
@@ -7449,13 +7458,13 @@
         <v>45022</v>
       </c>
       <c r="G61" s="24" t="s">
-        <v>393</v>
+        <v>361</v>
       </c>
       <c r="H61" s="24" t="s">
-        <v>392</v>
+        <v>360</v>
       </c>
       <c r="I61" s="24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J61" s="25" t="s">
         <v>68</v>
@@ -7474,7 +7483,7 @@
         <v>172</v>
       </c>
       <c r="P61" s="25" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="Q61" s="25"/>
       <c r="R61" s="26"/>
@@ -7494,7 +7503,7 @@
         <v>52</v>
       </c>
       <c r="D62" s="21" t="s">
-        <v>344</v>
+        <v>312</v>
       </c>
       <c r="E62" s="22" t="s">
         <v>66</v>
@@ -7503,13 +7512,13 @@
         <v>45022</v>
       </c>
       <c r="G62" s="24" t="s">
-        <v>394</v>
+        <v>362</v>
       </c>
       <c r="H62" s="24" t="s">
-        <v>395</v>
+        <v>363</v>
       </c>
       <c r="I62" s="24" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="J62" s="25" t="s">
         <v>68</v>
@@ -7528,7 +7537,7 @@
         <v>172</v>
       </c>
       <c r="P62" s="25" t="s">
-        <v>342</v>
+        <v>310</v>
       </c>
       <c r="Q62" s="25"/>
       <c r="R62" s="26"/>
@@ -7548,7 +7557,7 @@
         <v>52</v>
       </c>
       <c r="D63" s="21" t="s">
-        <v>345</v>
+        <v>313</v>
       </c>
       <c r="E63" s="22" t="s">
         <v>67</v>
@@ -7574,7 +7583,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="64" spans="1:20" ht="255.75" thickBot="1">
+    <row r="64" spans="1:20" ht="300.75" thickBot="1">
       <c r="A64" s="20">
         <v>147</v>
       </c>
@@ -7585,22 +7594,22 @@
         <v>52</v>
       </c>
       <c r="D64" s="21" t="s">
-        <v>346</v>
+        <v>314</v>
       </c>
       <c r="E64" s="22" t="s">
-        <v>347</v>
-      </c>
-      <c r="F64" s="23">
-        <v>45022</v>
-      </c>
-      <c r="G64" s="24" t="s">
-        <v>396</v>
-      </c>
-      <c r="H64" s="24" t="s">
-        <v>397</v>
+        <v>315</v>
+      </c>
+      <c r="F64" s="33">
+        <v>45034</v>
+      </c>
+      <c r="G64" s="36" t="s">
+        <v>440</v>
+      </c>
+      <c r="H64" s="36" t="s">
+        <v>441</v>
       </c>
       <c r="I64" s="24" t="s">
-        <v>398</v>
+        <v>442</v>
       </c>
       <c r="J64" s="25" t="s">
         <v>68</v>
@@ -7628,7 +7637,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="65" spans="1:20" ht="255.75" thickBot="1">
+    <row r="65" spans="1:20" ht="300.75" thickBot="1">
       <c r="A65" s="20">
         <v>148</v>
       </c>
@@ -7639,22 +7648,22 @@
         <v>52</v>
       </c>
       <c r="D65" s="21" t="s">
-        <v>348</v>
+        <v>316</v>
       </c>
       <c r="E65" s="22" t="s">
-        <v>349</v>
-      </c>
-      <c r="F65" s="23">
-        <v>45022</v>
-      </c>
-      <c r="G65" s="24" t="s">
-        <v>399</v>
-      </c>
-      <c r="H65" s="24" t="s">
-        <v>400</v>
+        <v>317</v>
+      </c>
+      <c r="F65" s="33">
+        <v>45034</v>
+      </c>
+      <c r="G65" s="36" t="s">
+        <v>445</v>
+      </c>
+      <c r="H65" s="36" t="s">
+        <v>443</v>
       </c>
       <c r="I65" s="24" t="s">
-        <v>401</v>
+        <v>444</v>
       </c>
       <c r="J65" s="25" t="s">
         <v>68</v>
@@ -7682,7 +7691,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="66" spans="1:20" ht="255.75" thickBot="1">
+    <row r="66" spans="1:20" ht="300.75" thickBot="1">
       <c r="A66" s="20">
         <v>149</v>
       </c>
@@ -7693,22 +7702,22 @@
         <v>52</v>
       </c>
       <c r="D66" s="21" t="s">
-        <v>350</v>
+        <v>318</v>
       </c>
       <c r="E66" s="22" t="s">
-        <v>351</v>
-      </c>
-      <c r="F66" s="23">
-        <v>45022</v>
-      </c>
-      <c r="G66" s="24" t="s">
-        <v>402</v>
+        <v>319</v>
+      </c>
+      <c r="F66" s="33">
+        <v>45034</v>
+      </c>
+      <c r="G66" s="36" t="s">
+        <v>448</v>
       </c>
       <c r="H66" s="24" t="s">
-        <v>403</v>
+        <v>446</v>
       </c>
       <c r="I66" s="24" t="s">
-        <v>404</v>
+        <v>447</v>
       </c>
       <c r="J66" s="25" t="s">
         <v>68</v>
@@ -7736,7 +7745,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="67" spans="1:20" ht="255.75" thickBot="1">
+    <row r="67" spans="1:20" ht="300.75" thickBot="1">
       <c r="A67" s="20">
         <v>150</v>
       </c>
@@ -7747,22 +7756,22 @@
         <v>52</v>
       </c>
       <c r="D67" s="21" t="s">
-        <v>352</v>
+        <v>320</v>
       </c>
       <c r="E67" s="22" t="s">
-        <v>353</v>
-      </c>
-      <c r="F67" s="23">
-        <v>45022</v>
-      </c>
-      <c r="G67" s="24" t="s">
-        <v>405</v>
+        <v>321</v>
+      </c>
+      <c r="F67" s="33">
+        <v>45034</v>
+      </c>
+      <c r="G67" s="36" t="s">
+        <v>450</v>
       </c>
       <c r="H67" s="24" t="s">
-        <v>406</v>
+        <v>449</v>
       </c>
       <c r="I67" s="24" t="s">
-        <v>407</v>
+        <v>451</v>
       </c>
       <c r="J67" s="25" t="s">
         <v>68</v>
@@ -7790,7 +7799,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="68" spans="1:20" ht="195.75" thickBot="1">
+    <row r="68" spans="1:20" ht="210.75" thickBot="1">
       <c r="A68" s="20">
         <v>151</v>
       </c>
@@ -7801,10 +7810,10 @@
         <v>52</v>
       </c>
       <c r="D68" s="21" t="s">
-        <v>354</v>
+        <v>322</v>
       </c>
       <c r="E68" s="22" t="s">
-        <v>355</v>
+        <v>323</v>
       </c>
       <c r="F68" s="23"/>
       <c r="G68" s="24"/>
@@ -7841,10 +7850,10 @@
         <v>52</v>
       </c>
       <c r="D69" s="21" t="s">
-        <v>356</v>
+        <v>324</v>
       </c>
       <c r="E69" s="22" t="s">
-        <v>357</v>
+        <v>325</v>
       </c>
       <c r="F69" s="23"/>
       <c r="G69" s="24"/>
@@ -7881,22 +7890,22 @@
         <v>52</v>
       </c>
       <c r="D70" s="21" t="s">
-        <v>358</v>
+        <v>326</v>
       </c>
       <c r="E70" s="22" t="s">
-        <v>359</v>
+        <v>327</v>
       </c>
       <c r="F70" s="23">
         <v>45022</v>
       </c>
       <c r="G70" s="24" t="s">
-        <v>408</v>
+        <v>364</v>
       </c>
       <c r="H70" s="24" t="s">
-        <v>409</v>
+        <v>365</v>
       </c>
       <c r="I70" s="24" t="s">
-        <v>410</v>
+        <v>366</v>
       </c>
       <c r="J70" s="25" t="s">
         <v>68</v>
@@ -7935,22 +7944,22 @@
         <v>52</v>
       </c>
       <c r="D71" s="21" t="s">
-        <v>360</v>
+        <v>328</v>
       </c>
       <c r="E71" s="22" t="s">
-        <v>361</v>
+        <v>329</v>
       </c>
       <c r="F71" s="23">
         <v>45022</v>
       </c>
       <c r="G71" s="24" t="s">
-        <v>411</v>
+        <v>367</v>
       </c>
       <c r="H71" s="24" t="s">
-        <v>412</v>
+        <v>368</v>
       </c>
       <c r="I71" s="24" t="s">
-        <v>413</v>
+        <v>369</v>
       </c>
       <c r="J71" s="25" t="s">
         <v>68</v>
@@ -7989,22 +7998,22 @@
         <v>52</v>
       </c>
       <c r="D72" s="21" t="s">
-        <v>362</v>
+        <v>330</v>
       </c>
       <c r="E72" s="22" t="s">
-        <v>363</v>
+        <v>331</v>
       </c>
       <c r="F72" s="23">
         <v>45022</v>
       </c>
       <c r="G72" s="24" t="s">
-        <v>414</v>
+        <v>370</v>
       </c>
       <c r="H72" s="24" t="s">
-        <v>415</v>
+        <v>371</v>
       </c>
       <c r="I72" s="24" t="s">
-        <v>416</v>
+        <v>372</v>
       </c>
       <c r="J72" s="25" t="s">
         <v>68</v>
@@ -8043,10 +8052,10 @@
         <v>52</v>
       </c>
       <c r="D73" s="21" t="s">
-        <v>364</v>
+        <v>332</v>
       </c>
       <c r="E73" s="22" t="s">
-        <v>365</v>
+        <v>333</v>
       </c>
       <c r="F73" s="23"/>
       <c r="G73" s="24"/>
@@ -8083,22 +8092,22 @@
         <v>52</v>
       </c>
       <c r="D74" s="21" t="s">
-        <v>366</v>
+        <v>334</v>
       </c>
       <c r="E74" s="22" t="s">
-        <v>367</v>
+        <v>335</v>
       </c>
       <c r="F74" s="23">
         <v>45022</v>
       </c>
       <c r="G74" s="24" t="s">
-        <v>417</v>
+        <v>373</v>
       </c>
       <c r="H74" s="24" t="s">
-        <v>418</v>
+        <v>374</v>
       </c>
       <c r="I74" s="24" t="s">
-        <v>419</v>
+        <v>375</v>
       </c>
       <c r="J74" s="25" t="s">
         <v>68</v>
@@ -8137,22 +8146,22 @@
         <v>52</v>
       </c>
       <c r="D75" s="21" t="s">
-        <v>368</v>
+        <v>336</v>
       </c>
       <c r="E75" s="22" t="s">
-        <v>369</v>
+        <v>337</v>
       </c>
       <c r="F75" s="23">
         <v>45022</v>
       </c>
       <c r="G75" s="24" t="s">
-        <v>420</v>
+        <v>376</v>
       </c>
       <c r="H75" s="24" t="s">
-        <v>421</v>
+        <v>377</v>
       </c>
       <c r="I75" s="24" t="s">
-        <v>422</v>
+        <v>378</v>
       </c>
       <c r="J75" s="25" t="s">
         <v>68</v>
@@ -8191,22 +8200,22 @@
         <v>52</v>
       </c>
       <c r="D76" s="21" t="s">
-        <v>370</v>
+        <v>338</v>
       </c>
       <c r="E76" s="22" t="s">
-        <v>371</v>
+        <v>339</v>
       </c>
       <c r="F76" s="23">
         <v>45022</v>
       </c>
       <c r="G76" s="24" t="s">
-        <v>423</v>
+        <v>379</v>
       </c>
       <c r="H76" s="24" t="s">
-        <v>424</v>
+        <v>380</v>
       </c>
       <c r="I76" s="24" t="s">
-        <v>425</v>
+        <v>381</v>
       </c>
       <c r="J76" s="25" t="s">
         <v>68</v>
@@ -8245,22 +8254,22 @@
         <v>52</v>
       </c>
       <c r="D77" s="21" t="s">
-        <v>372</v>
+        <v>340</v>
       </c>
       <c r="E77" s="22" t="s">
-        <v>373</v>
+        <v>341</v>
       </c>
       <c r="F77" s="23">
         <v>45022</v>
       </c>
       <c r="G77" s="24" t="s">
-        <v>426</v>
+        <v>382</v>
       </c>
       <c r="H77" s="24" t="s">
-        <v>427</v>
+        <v>383</v>
       </c>
       <c r="I77" s="24" t="s">
-        <v>428</v>
+        <v>384</v>
       </c>
       <c r="J77" s="25" t="s">
         <v>68</v>
@@ -8299,10 +8308,10 @@
         <v>52</v>
       </c>
       <c r="D78" s="21" t="s">
-        <v>374</v>
+        <v>342</v>
       </c>
       <c r="E78" s="22" t="s">
-        <v>375</v>
+        <v>343</v>
       </c>
       <c r="F78" s="23"/>
       <c r="G78" s="24"/>
@@ -8312,7 +8321,7 @@
         <v>172</v>
       </c>
       <c r="K78" s="25" t="s">
-        <v>450</v>
+        <v>406</v>
       </c>
       <c r="L78" s="25"/>
       <c r="M78" s="25"/>
@@ -8339,22 +8348,22 @@
         <v>52</v>
       </c>
       <c r="D79" s="21" t="s">
-        <v>376</v>
+        <v>344</v>
       </c>
       <c r="E79" s="22" t="s">
-        <v>377</v>
+        <v>345</v>
       </c>
       <c r="F79" s="23">
         <v>45022</v>
       </c>
       <c r="G79" s="24" t="s">
-        <v>429</v>
+        <v>385</v>
       </c>
       <c r="H79" s="24" t="s">
-        <v>430</v>
+        <v>386</v>
       </c>
       <c r="I79" s="24" t="s">
-        <v>431</v>
+        <v>387</v>
       </c>
       <c r="J79" s="25" t="s">
         <v>68</v>
@@ -8393,22 +8402,22 @@
         <v>52</v>
       </c>
       <c r="D80" s="21" t="s">
-        <v>378</v>
+        <v>346</v>
       </c>
       <c r="E80" s="22" t="s">
-        <v>379</v>
+        <v>347</v>
       </c>
       <c r="F80" s="23">
         <v>45022</v>
       </c>
       <c r="G80" s="24" t="s">
-        <v>432</v>
+        <v>388</v>
       </c>
       <c r="H80" s="24" t="s">
-        <v>433</v>
+        <v>389</v>
       </c>
       <c r="I80" s="24" t="s">
-        <v>434</v>
+        <v>390</v>
       </c>
       <c r="J80" s="25" t="s">
         <v>68</v>
@@ -8447,22 +8456,22 @@
         <v>52</v>
       </c>
       <c r="D81" s="21" t="s">
-        <v>380</v>
+        <v>348</v>
       </c>
       <c r="E81" s="22" t="s">
-        <v>381</v>
+        <v>349</v>
       </c>
       <c r="F81" s="23">
         <v>45022</v>
       </c>
       <c r="G81" s="24" t="s">
-        <v>435</v>
+        <v>391</v>
       </c>
       <c r="H81" s="24" t="s">
-        <v>436</v>
+        <v>392</v>
       </c>
       <c r="I81" s="24" t="s">
-        <v>437</v>
+        <v>393</v>
       </c>
       <c r="J81" s="25" t="s">
         <v>68</v>
@@ -8501,22 +8510,22 @@
         <v>52</v>
       </c>
       <c r="D82" s="21" t="s">
-        <v>382</v>
+        <v>350</v>
       </c>
       <c r="E82" s="22" t="s">
-        <v>383</v>
+        <v>351</v>
       </c>
       <c r="F82" s="23">
         <v>45022</v>
       </c>
       <c r="G82" s="24" t="s">
-        <v>438</v>
+        <v>394</v>
       </c>
       <c r="H82" s="24" t="s">
-        <v>439</v>
+        <v>395</v>
       </c>
       <c r="I82" s="24" t="s">
-        <v>440</v>
+        <v>396</v>
       </c>
       <c r="J82" s="25" t="s">
         <v>68</v>
@@ -8555,22 +8564,22 @@
         <v>52</v>
       </c>
       <c r="D83" s="21" t="s">
-        <v>384</v>
+        <v>352</v>
       </c>
       <c r="E83" s="22" t="s">
-        <v>385</v>
+        <v>353</v>
       </c>
       <c r="F83" s="23">
         <v>45022</v>
       </c>
       <c r="G83" s="24" t="s">
-        <v>441</v>
+        <v>397</v>
       </c>
       <c r="H83" s="24" t="s">
-        <v>442</v>
+        <v>398</v>
       </c>
       <c r="I83" s="24" t="s">
-        <v>443</v>
+        <v>399</v>
       </c>
       <c r="J83" s="25" t="s">
         <v>68</v>
@@ -8609,22 +8618,22 @@
         <v>52</v>
       </c>
       <c r="D84" s="21" t="s">
-        <v>386</v>
+        <v>354</v>
       </c>
       <c r="E84" s="22" t="s">
-        <v>387</v>
+        <v>355</v>
       </c>
       <c r="F84" s="23">
         <v>45022</v>
       </c>
       <c r="G84" s="24" t="s">
-        <v>444</v>
+        <v>400</v>
       </c>
       <c r="H84" s="24" t="s">
-        <v>445</v>
+        <v>401</v>
       </c>
       <c r="I84" s="24" t="s">
-        <v>446</v>
+        <v>402</v>
       </c>
       <c r="J84" s="25" t="s">
         <v>68</v>
@@ -8663,22 +8672,22 @@
         <v>52</v>
       </c>
       <c r="D85" s="21" t="s">
-        <v>388</v>
+        <v>356</v>
       </c>
       <c r="E85" s="22" t="s">
-        <v>389</v>
+        <v>357</v>
       </c>
       <c r="F85" s="23">
         <v>45022</v>
       </c>
       <c r="G85" s="24" t="s">
-        <v>447</v>
+        <v>403</v>
       </c>
       <c r="H85" s="24" t="s">
-        <v>448</v>
+        <v>404</v>
       </c>
       <c r="I85" s="24" t="s">
-        <v>449</v>
+        <v>405</v>
       </c>
       <c r="J85" s="25" t="s">
         <v>68</v>
@@ -8717,10 +8726,10 @@
         <v>52</v>
       </c>
       <c r="D86" s="21" t="s">
-        <v>390</v>
+        <v>358</v>
       </c>
       <c r="E86" s="22" t="s">
-        <v>391</v>
+        <v>359</v>
       </c>
       <c r="F86" s="23"/>
       <c r="G86" s="24"/>
@@ -8730,7 +8739,7 @@
         <v>172</v>
       </c>
       <c r="K86" s="25" t="s">
-        <v>451</v>
+        <v>407</v>
       </c>
       <c r="L86" s="25"/>
       <c r="M86" s="25"/>

</xml_diff>

<commit_message>
sistemate segnalazioni 18 aprile 2023
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Devel\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\HERO\5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCFBAEC0-2CF5-4EDC-A9D6-75E2537AB34D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BBFE6D-9968-49C5-A2BB-4C5CE1D37692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="23070" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2132,9 +2132,6 @@
     <xf numFmtId="14" fontId="2" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="11" fontId="2" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
@@ -2166,14 +2163,17 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="20" fontId="2" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
     <xf numFmtId="14" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4634,10 +4634,10 @@
   <dimension ref="A1:T659"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B67" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G67" sqref="G67"/>
+      <selection pane="bottomRight" activeCell="I67" sqref="I67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4683,12 +4683,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="40" t="s">
+      <c r="A2" s="39" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="41"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="41"/>
+      <c r="B2" s="40"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="40"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4706,14 +4706,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="43" t="s">
+      <c r="A3" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="44"/>
-      <c r="C3" s="49" t="s">
+      <c r="B3" s="43"/>
+      <c r="C3" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="41"/>
+      <c r="D3" s="40"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4731,12 +4731,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="45"/>
-      <c r="B4" s="46"/>
-      <c r="C4" s="49" t="s">
+      <c r="A4" s="44"/>
+      <c r="B4" s="45"/>
+      <c r="C4" s="48" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="41"/>
+      <c r="D4" s="40"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4755,12 +4755,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="47"/>
-      <c r="B5" s="48"/>
-      <c r="C5" s="49" t="s">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="48" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="41"/>
+      <c r="D5" s="40"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4778,8 +4778,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="38"/>
-      <c r="B6" s="39"/>
+      <c r="A6" s="37"/>
+      <c r="B6" s="38"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4896,7 +4896,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:20" ht="225.75" thickBot="1">
+    <row r="10" spans="1:20" ht="270.75" thickBot="1">
       <c r="A10" s="20">
         <v>24</v>
       </c>
@@ -4915,13 +4915,13 @@
       <c r="F10" s="33">
         <v>45034</v>
       </c>
-      <c r="G10" s="51" t="s">
+      <c r="G10" s="49" t="s">
         <v>408</v>
       </c>
-      <c r="H10" s="50" t="s">
+      <c r="H10" s="51" t="s">
         <v>409</v>
       </c>
-      <c r="I10" s="34" t="s">
+      <c r="I10" s="49" t="s">
         <v>410</v>
       </c>
       <c r="J10" s="25" t="s">
@@ -4940,7 +4940,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="11" spans="1:20" ht="225.75" thickBot="1">
+    <row r="11" spans="1:20" ht="270.75" thickBot="1">
       <c r="A11" s="20">
         <v>25</v>
       </c>
@@ -4959,13 +4959,13 @@
       <c r="F11" s="33">
         <v>45034</v>
       </c>
-      <c r="G11" s="51" t="s">
+      <c r="G11" s="49" t="s">
         <v>411</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="35" t="s">
         <v>412</v>
       </c>
-      <c r="I11" s="36" t="s">
+      <c r="I11" s="35" t="s">
         <v>413</v>
       </c>
       <c r="J11" s="25" t="s">
@@ -4984,7 +4984,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="12" spans="1:20" ht="225.75" thickBot="1">
+    <row r="12" spans="1:20" ht="270.75" thickBot="1">
       <c r="A12" s="20">
         <v>26</v>
       </c>
@@ -5003,13 +5003,13 @@
       <c r="F12" s="33">
         <v>45034</v>
       </c>
-      <c r="G12" s="51" t="s">
+      <c r="G12" s="49" t="s">
         <v>414</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="I12" s="35" t="s">
         <v>416</v>
       </c>
       <c r="J12" s="25" t="s">
@@ -5028,7 +5028,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="13" spans="1:20" ht="225.75" thickBot="1">
+    <row r="13" spans="1:20" ht="270.75" thickBot="1">
       <c r="A13" s="20">
         <v>27</v>
       </c>
@@ -5047,13 +5047,13 @@
       <c r="F13" s="33">
         <v>45034</v>
       </c>
-      <c r="G13" s="51" t="s">
+      <c r="G13" s="49" t="s">
         <v>417</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="35" t="s">
         <v>418</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="I13" s="35" t="s">
         <v>419</v>
       </c>
       <c r="J13" s="25" t="s">
@@ -5072,7 +5072,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:20" ht="225.75" thickBot="1">
+    <row r="14" spans="1:20" ht="240.75" thickBot="1">
       <c r="A14" s="20">
         <v>35</v>
       </c>
@@ -5085,16 +5085,16 @@
       <c r="D14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="52" t="s">
+      <c r="E14" s="50" t="s">
         <v>64</v>
       </c>
       <c r="F14" s="33">
         <v>45034</v>
       </c>
-      <c r="G14" s="51" t="s">
+      <c r="G14" s="49" t="s">
         <v>421</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="35" t="s">
         <v>420</v>
       </c>
       <c r="I14" s="24" t="s">
@@ -5126,7 +5126,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="15" spans="1:20" ht="210.75" thickBot="1">
+    <row r="15" spans="1:20" ht="255.75" thickBot="1">
       <c r="A15" s="20">
         <v>43</v>
       </c>
@@ -5139,16 +5139,16 @@
       <c r="D15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="52" t="s">
+      <c r="E15" s="50" t="s">
         <v>66</v>
       </c>
       <c r="F15" s="33">
         <v>45034</v>
       </c>
-      <c r="G15" s="51" t="s">
+      <c r="G15" s="49" t="s">
         <v>423</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="35" t="s">
         <v>422</v>
       </c>
       <c r="I15" s="24" t="s">
@@ -5618,7 +5618,7 @@
       <c r="G25" s="24" t="s">
         <v>232</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="H25" s="34" t="s">
         <v>233</v>
       </c>
       <c r="I25" s="24" t="s">
@@ -6533,16 +6533,16 @@
       <c r="F42" s="33">
         <v>45034</v>
       </c>
-      <c r="G42" s="51" t="s">
+      <c r="G42" s="49" t="s">
         <v>426</v>
       </c>
-      <c r="H42" s="24" t="s">
+      <c r="H42" s="35" t="s">
         <v>424</v>
       </c>
-      <c r="I42" s="36" t="s">
+      <c r="I42" s="35" t="s">
         <v>425</v>
       </c>
-      <c r="J42" s="37" t="s">
+      <c r="J42" s="36" t="s">
         <v>68</v>
       </c>
       <c r="P42" s="25"/>
@@ -6572,13 +6572,13 @@
       <c r="F43" s="33">
         <v>45034</v>
       </c>
-      <c r="G43" s="36" t="s">
+      <c r="G43" s="35" t="s">
         <v>432</v>
       </c>
-      <c r="H43" s="24" t="s">
+      <c r="H43" s="35" t="s">
         <v>427</v>
       </c>
-      <c r="I43" s="36" t="s">
+      <c r="I43" s="35" t="s">
         <v>428</v>
       </c>
       <c r="J43" s="25" t="s">
@@ -6616,13 +6616,13 @@
       <c r="F44" s="33">
         <v>45034</v>
       </c>
-      <c r="G44" s="36" t="s">
+      <c r="G44" s="35" t="s">
         <v>431</v>
       </c>
-      <c r="H44" s="24" t="s">
+      <c r="H44" s="35" t="s">
         <v>429</v>
       </c>
-      <c r="I44" s="36" t="s">
+      <c r="I44" s="35" t="s">
         <v>430</v>
       </c>
       <c r="J44" s="25" t="s">
@@ -6660,13 +6660,13 @@
       <c r="F45" s="33">
         <v>45034</v>
       </c>
-      <c r="G45" s="36" t="s">
+      <c r="G45" s="35" t="s">
         <v>434</v>
       </c>
-      <c r="H45" s="35" t="s">
+      <c r="H45" s="52" t="s">
         <v>433</v>
       </c>
-      <c r="I45" s="24" t="s">
+      <c r="I45" s="35" t="s">
         <v>435</v>
       </c>
       <c r="J45" s="25" t="s">
@@ -6704,10 +6704,10 @@
       <c r="F46" s="33">
         <v>45034</v>
       </c>
-      <c r="G46" s="36" t="s">
+      <c r="G46" s="35" t="s">
         <v>437</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="H46" s="35" t="s">
         <v>436</v>
       </c>
       <c r="I46" s="24" t="s">
@@ -6752,16 +6752,16 @@
       <c r="D47" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="E47" s="52" t="s">
+      <c r="E47" s="50" t="s">
         <v>66</v>
       </c>
       <c r="F47" s="33">
         <v>45034</v>
       </c>
-      <c r="G47" s="36" t="s">
+      <c r="G47" s="35" t="s">
         <v>439</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="35" t="s">
         <v>438</v>
       </c>
       <c r="I47" s="24" t="s">
@@ -6932,7 +6932,7 @@
       <c r="F51" s="33">
         <v>45008</v>
       </c>
-      <c r="G51" s="36" t="s">
+      <c r="G51" s="35" t="s">
         <v>284</v>
       </c>
       <c r="H51" s="24" t="s">
@@ -7187,7 +7187,7 @@
       <c r="F56" s="33">
         <v>45008</v>
       </c>
-      <c r="G56" s="36" t="s">
+      <c r="G56" s="35" t="s">
         <v>295</v>
       </c>
       <c r="H56" s="24" t="s">
@@ -7602,13 +7602,13 @@
       <c r="F64" s="33">
         <v>45034</v>
       </c>
-      <c r="G64" s="36" t="s">
+      <c r="G64" s="35" t="s">
         <v>440</v>
       </c>
-      <c r="H64" s="36" t="s">
+      <c r="H64" s="35" t="s">
         <v>441</v>
       </c>
-      <c r="I64" s="24" t="s">
+      <c r="I64" s="35" t="s">
         <v>442</v>
       </c>
       <c r="J64" s="25" t="s">
@@ -7656,13 +7656,13 @@
       <c r="F65" s="33">
         <v>45034</v>
       </c>
-      <c r="G65" s="36" t="s">
+      <c r="G65" s="35" t="s">
         <v>445</v>
       </c>
-      <c r="H65" s="36" t="s">
+      <c r="H65" s="35" t="s">
         <v>443</v>
       </c>
-      <c r="I65" s="24" t="s">
+      <c r="I65" s="35" t="s">
         <v>444</v>
       </c>
       <c r="J65" s="25" t="s">
@@ -7710,13 +7710,13 @@
       <c r="F66" s="33">
         <v>45034</v>
       </c>
-      <c r="G66" s="36" t="s">
+      <c r="G66" s="35" t="s">
         <v>448</v>
       </c>
-      <c r="H66" s="24" t="s">
+      <c r="H66" s="35" t="s">
         <v>446</v>
       </c>
-      <c r="I66" s="24" t="s">
+      <c r="I66" s="35" t="s">
         <v>447</v>
       </c>
       <c r="J66" s="25" t="s">
@@ -7764,13 +7764,13 @@
       <c r="F67" s="33">
         <v>45034</v>
       </c>
-      <c r="G67" s="36" t="s">
+      <c r="G67" s="35" t="s">
         <v>450</v>
       </c>
-      <c r="H67" s="24" t="s">
+      <c r="H67" s="35" t="s">
         <v>449</v>
       </c>
-      <c r="I67" s="24" t="s">
+      <c r="I67" s="35" t="s">
         <v>451</v>
       </c>
       <c r="J67" s="25" t="s">

</xml_diff>

<commit_message>
sistemate segnalazioni 21 aprile 2023
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Devel\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\HERO\5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{89BBFE6D-9968-49C5-A2BB-4C5CE1D37692}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0C26066-DFC5-4BA0-9E5A-8B1401034470}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="23070" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1605,15 +1605,6 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.4c083e2fd0252d4d741c1d91e37f7a08faaba81283a736d5d4c1062614b5c67d.59bfc4ecb6^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>2023-04-18T15:14:57Z</t>
-  </si>
-  <si>
-    <t>47d1566689772b77</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.c4e3b0df69c3aa128a9f26f4a492453e199b680dff77957040ee12927f49cd33.99499b9e77^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
     <t>3e41c3314382acb7</t>
   </si>
   <si>
@@ -1668,12 +1659,6 @@
     <t>2023-04-18T15:36:12Z</t>
   </si>
   <si>
-    <t>0f6324059b71374a</t>
-  </si>
-  <si>
-    <t>2023-04-18T15:40:46Z</t>
-  </si>
-  <si>
     <t>2023-04-18T15:47:25Z</t>
   </si>
   <si>
@@ -1683,31 +1668,46 @@
     <t>2.16.840.1.113883.2.9.2.150.4.4.0bada2628a915e683ae1850e263ec2587a0d5d1042803419829fc922dec26c5b.5244963f69^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
   </si>
   <si>
-    <t>f79823d2fc5ea9d3</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.9d2810e4b8d89b76fcd3d3a20fb907bf12b4359d15910985725131df945e509b.39c0b575bc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-18T16:03:53Z</t>
-  </si>
-  <si>
-    <t>eddc22525d89a0b5</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.330734ed8ddfaee1745e7cbb033f2e0ae3001fbbc75497e5e4efb1f797aa19dc.edafa62317^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-18T16:41:32Z</t>
-  </si>
-  <si>
-    <t>e590df00ddc4a306</t>
-  </si>
-  <si>
-    <t>2023-04-18T16:43:17Z</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.934167a59c9f6667655d91d04807f0b8b2283f57358e23960660542ea9ba4327.9f7f91b5f0^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+    <t>2023-04-21T18:16:22Z</t>
+  </si>
+  <si>
+    <t>bc758664b7b979c4</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.c4e3b0df69c3aa128a9f26f4a492453e199b680dff77957040ee12927f49cd33.64fef27aa4^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>4004674af651dcaa</t>
+  </si>
+  <si>
+    <t>2023-04-21T18:20:15Z</t>
+  </si>
+  <si>
+    <t>1478da74656d93fa</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.9d2810e4b8d89b76fcd3d3a20fb907bf12b4359d15910985725131df945e509b.27e66300dc^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-21T18:33:10Z</t>
+  </si>
+  <si>
+    <t>98ce35bbd4f47cdf</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.330734ed8ddfaee1745e7cbb033f2e0ae3001fbbc75497e5e4efb1f797aa19dc.e21627db4b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-21T18:40:58Z</t>
+  </si>
+  <si>
+    <t>21c775a9ff02c75a</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.934167a59c9f6667655d91d04807f0b8b2283f57358e23960660542ea9ba4327.671eee0e02^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-21T18:55:13Z</t>
   </si>
 </sst>
 </file>
@@ -2141,6 +2141,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
+    <xf numFmtId="11" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -2162,18 +2174,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="9" fillId="4" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="11" fontId="9" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1" readingOrder="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -4634,10 +4634,10 @@
   <dimension ref="A1:T659"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="C86" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="C67" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="I67" sqref="I67"/>
+      <selection pane="bottomRight" activeCell="H67" sqref="H67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -4683,12 +4683,12 @@
       <c r="T1" s="15"/>
     </row>
     <row r="2" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A2" s="39" t="s">
+      <c r="A2" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
-      <c r="D2" s="40"/>
+      <c r="B2" s="44"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="44"/>
       <c r="F2" s="12"/>
       <c r="G2" s="12"/>
       <c r="H2" s="12"/>
@@ -4706,14 +4706,14 @@
       <c r="T2" s="15"/>
     </row>
     <row r="3" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A3" s="42" t="s">
+      <c r="A3" s="46" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="43"/>
-      <c r="C3" s="48" t="s">
+      <c r="B3" s="47"/>
+      <c r="C3" s="52" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="40"/>
+      <c r="D3" s="44"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -4731,12 +4731,12 @@
       <c r="T3" s="15"/>
     </row>
     <row r="4" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A4" s="44"/>
-      <c r="B4" s="45"/>
-      <c r="C4" s="48" t="s">
+      <c r="A4" s="48"/>
+      <c r="B4" s="49"/>
+      <c r="C4" s="52" t="s">
         <v>174</v>
       </c>
-      <c r="D4" s="40"/>
+      <c r="D4" s="44"/>
       <c r="E4" s="4"/>
       <c r="F4" s="12"/>
       <c r="G4" s="12"/>
@@ -4755,12 +4755,12 @@
       <c r="T4" s="15"/>
     </row>
     <row r="5" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A5" s="46"/>
-      <c r="B5" s="47"/>
-      <c r="C5" s="48" t="s">
+      <c r="A5" s="50"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="52" t="s">
         <v>175</v>
       </c>
-      <c r="D5" s="40"/>
+      <c r="D5" s="44"/>
       <c r="F5" s="12"/>
       <c r="G5" s="12"/>
       <c r="H5" s="12"/>
@@ -4778,8 +4778,8 @@
       <c r="T5" s="15"/>
     </row>
     <row r="6" spans="1:20" ht="14.25" customHeight="1">
-      <c r="A6" s="37"/>
-      <c r="B6" s="38"/>
+      <c r="A6" s="41"/>
+      <c r="B6" s="42"/>
       <c r="C6" s="16"/>
       <c r="F6" s="12"/>
       <c r="G6" s="12"/>
@@ -4915,13 +4915,13 @@
       <c r="F10" s="33">
         <v>45034</v>
       </c>
-      <c r="G10" s="49" t="s">
+      <c r="G10" s="37" t="s">
         <v>408</v>
       </c>
-      <c r="H10" s="51" t="s">
+      <c r="H10" s="39" t="s">
         <v>409</v>
       </c>
-      <c r="I10" s="49" t="s">
+      <c r="I10" s="37" t="s">
         <v>410</v>
       </c>
       <c r="J10" s="25" t="s">
@@ -4959,7 +4959,7 @@
       <c r="F11" s="33">
         <v>45034</v>
       </c>
-      <c r="G11" s="49" t="s">
+      <c r="G11" s="37" t="s">
         <v>411</v>
       </c>
       <c r="H11" s="35" t="s">
@@ -5003,7 +5003,7 @@
       <c r="F12" s="33">
         <v>45034</v>
       </c>
-      <c r="G12" s="49" t="s">
+      <c r="G12" s="37" t="s">
         <v>414</v>
       </c>
       <c r="H12" s="35" t="s">
@@ -5045,16 +5045,16 @@
         <v>62</v>
       </c>
       <c r="F13" s="33">
-        <v>45034</v>
-      </c>
-      <c r="G13" s="49" t="s">
-        <v>417</v>
+        <v>45037</v>
+      </c>
+      <c r="G13" s="37" t="s">
+        <v>438</v>
       </c>
       <c r="H13" s="35" t="s">
-        <v>418</v>
+        <v>439</v>
       </c>
       <c r="I13" s="35" t="s">
-        <v>419</v>
+        <v>440</v>
       </c>
       <c r="J13" s="25" t="s">
         <v>68</v>
@@ -5085,17 +5085,17 @@
       <c r="D14" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E14" s="50" t="s">
+      <c r="E14" s="38" t="s">
         <v>64</v>
       </c>
       <c r="F14" s="33">
         <v>45034</v>
       </c>
-      <c r="G14" s="49" t="s">
-        <v>421</v>
+      <c r="G14" s="37" t="s">
+        <v>418</v>
       </c>
       <c r="H14" s="35" t="s">
-        <v>420</v>
+        <v>417</v>
       </c>
       <c r="I14" s="24" t="s">
         <v>219</v>
@@ -5139,17 +5139,17 @@
       <c r="D15" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="50" t="s">
+      <c r="E15" s="38" t="s">
         <v>66</v>
       </c>
       <c r="F15" s="33">
         <v>45034</v>
       </c>
-      <c r="G15" s="49" t="s">
-        <v>423</v>
+      <c r="G15" s="37" t="s">
+        <v>420</v>
       </c>
       <c r="H15" s="35" t="s">
-        <v>422</v>
+        <v>419</v>
       </c>
       <c r="I15" s="24" t="s">
         <v>219</v>
@@ -5220,7 +5220,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="17" spans="1:20" ht="180.75" thickBot="1">
+    <row r="17" spans="1:20" ht="210.75" thickBot="1">
       <c r="A17" s="20">
         <v>122</v>
       </c>
@@ -5260,7 +5260,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="18" spans="1:20" ht="180.75" thickBot="1">
+    <row r="18" spans="1:20" ht="210.75" thickBot="1">
       <c r="A18" s="20">
         <v>123</v>
       </c>
@@ -5300,7 +5300,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="1:20" ht="180.75" thickBot="1">
+    <row r="19" spans="1:20" ht="210.75" thickBot="1">
       <c r="A19" s="20">
         <v>124</v>
       </c>
@@ -5354,7 +5354,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="20" spans="1:20" ht="195.75" thickBot="1">
+    <row r="20" spans="1:20" ht="225.75" thickBot="1">
       <c r="A20" s="20">
         <v>125</v>
       </c>
@@ -5408,7 +5408,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="21" spans="1:20" ht="180.75" thickBot="1">
+    <row r="21" spans="1:20" ht="210.75" thickBot="1">
       <c r="A21" s="20">
         <v>126</v>
       </c>
@@ -5462,7 +5462,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="22" spans="1:20" ht="180.75" thickBot="1">
+    <row r="22" spans="1:20" ht="225.75" thickBot="1">
       <c r="A22" s="20">
         <v>127</v>
       </c>
@@ -5502,7 +5502,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:20" ht="180.75" thickBot="1">
+    <row r="23" spans="1:20" ht="210.75" thickBot="1">
       <c r="A23" s="20">
         <v>128</v>
       </c>
@@ -5556,7 +5556,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:20" ht="195.75" thickBot="1">
+    <row r="24" spans="1:20" ht="225.75" thickBot="1">
       <c r="A24" s="20">
         <v>129</v>
       </c>
@@ -5596,7 +5596,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="25" spans="1:20" ht="180.75" thickBot="1">
+    <row r="25" spans="1:20" ht="210.75" thickBot="1">
       <c r="A25" s="20">
         <v>130</v>
       </c>
@@ -5650,7 +5650,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="26" spans="1:20" ht="180.75" thickBot="1">
+    <row r="26" spans="1:20" ht="210.75" thickBot="1">
       <c r="A26" s="20">
         <v>131</v>
       </c>
@@ -5704,7 +5704,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="1:20" ht="180.75" thickBot="1">
+    <row r="27" spans="1:20" ht="210.75" thickBot="1">
       <c r="A27" s="20">
         <v>132</v>
       </c>
@@ -5758,7 +5758,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:20" ht="195.75" thickBot="1">
+    <row r="28" spans="1:20" ht="225.75" thickBot="1">
       <c r="A28" s="20">
         <v>133</v>
       </c>
@@ -5812,7 +5812,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="29" spans="1:20" ht="180.75" thickBot="1">
+    <row r="29" spans="1:20" ht="210.75" thickBot="1">
       <c r="A29" s="20">
         <v>134</v>
       </c>
@@ -5866,7 +5866,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="30" spans="1:20" ht="180.75" thickBot="1">
+    <row r="30" spans="1:20" ht="210.75" thickBot="1">
       <c r="A30" s="20">
         <v>135</v>
       </c>
@@ -5920,7 +5920,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="31" spans="1:20" ht="180.75" thickBot="1">
+    <row r="31" spans="1:20" ht="210.75" thickBot="1">
       <c r="A31" s="20">
         <v>136</v>
       </c>
@@ -5974,7 +5974,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="32" spans="1:20" ht="195.75" thickBot="1">
+    <row r="32" spans="1:20" ht="225.75" thickBot="1">
       <c r="A32" s="20">
         <v>137</v>
       </c>
@@ -6028,7 +6028,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="33" spans="1:20" ht="180.75" thickBot="1">
+    <row r="33" spans="1:20" ht="210.75" thickBot="1">
       <c r="A33" s="20">
         <v>138</v>
       </c>
@@ -6082,7 +6082,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="34" spans="1:20" ht="180.75" thickBot="1">
+    <row r="34" spans="1:20" ht="210.75" thickBot="1">
       <c r="A34" s="20">
         <v>139</v>
       </c>
@@ -6136,7 +6136,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="35" spans="1:20" ht="180.75" thickBot="1">
+    <row r="35" spans="1:20" ht="210.75" thickBot="1">
       <c r="A35" s="20">
         <v>140</v>
       </c>
@@ -6190,7 +6190,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="36" spans="1:20" ht="195.75" thickBot="1">
+    <row r="36" spans="1:20" ht="225.75" thickBot="1">
       <c r="A36" s="20">
         <v>141</v>
       </c>
@@ -6244,7 +6244,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="37" spans="1:20" ht="180.75" thickBot="1">
+    <row r="37" spans="1:20" ht="225.75" thickBot="1">
       <c r="A37" s="20">
         <v>142</v>
       </c>
@@ -6298,7 +6298,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="38" spans="1:20" ht="180.75" thickBot="1">
+    <row r="38" spans="1:20" ht="225.75" thickBot="1">
       <c r="A38" s="20">
         <v>143</v>
       </c>
@@ -6352,7 +6352,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="39" spans="1:20" ht="180.75" thickBot="1">
+    <row r="39" spans="1:20" ht="225.75" thickBot="1">
       <c r="A39" s="20">
         <v>144</v>
       </c>
@@ -6406,7 +6406,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="40" spans="1:20" ht="195.75" thickBot="1">
+    <row r="40" spans="1:20" ht="240.75" thickBot="1">
       <c r="A40" s="20">
         <v>145</v>
       </c>
@@ -6533,14 +6533,14 @@
       <c r="F42" s="33">
         <v>45034</v>
       </c>
-      <c r="G42" s="49" t="s">
-        <v>426</v>
+      <c r="G42" s="37" t="s">
+        <v>423</v>
       </c>
       <c r="H42" s="35" t="s">
-        <v>424</v>
+        <v>421</v>
       </c>
       <c r="I42" s="35" t="s">
-        <v>425</v>
+        <v>422</v>
       </c>
       <c r="J42" s="36" t="s">
         <v>68</v>
@@ -6573,13 +6573,13 @@
         <v>45034</v>
       </c>
       <c r="G43" s="35" t="s">
-        <v>432</v>
+        <v>429</v>
       </c>
       <c r="H43" s="35" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="I43" s="35" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
       <c r="J43" s="25" t="s">
         <v>68</v>
@@ -6617,13 +6617,13 @@
         <v>45034</v>
       </c>
       <c r="G44" s="35" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="H44" s="35" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="I44" s="35" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
       <c r="J44" s="25" t="s">
         <v>68</v>
@@ -6661,13 +6661,13 @@
         <v>45034</v>
       </c>
       <c r="G45" s="35" t="s">
-        <v>434</v>
-      </c>
-      <c r="H45" s="52" t="s">
-        <v>433</v>
+        <v>431</v>
+      </c>
+      <c r="H45" s="40" t="s">
+        <v>430</v>
       </c>
       <c r="I45" s="35" t="s">
-        <v>435</v>
+        <v>432</v>
       </c>
       <c r="J45" s="25" t="s">
         <v>68</v>
@@ -6705,10 +6705,10 @@
         <v>45034</v>
       </c>
       <c r="G46" s="35" t="s">
-        <v>437</v>
+        <v>434</v>
       </c>
       <c r="H46" s="35" t="s">
-        <v>436</v>
+        <v>433</v>
       </c>
       <c r="I46" s="24" t="s">
         <v>219</v>
@@ -6752,17 +6752,17 @@
       <c r="D47" s="21" t="s">
         <v>185</v>
       </c>
-      <c r="E47" s="50" t="s">
+      <c r="E47" s="38" t="s">
         <v>66</v>
       </c>
       <c r="F47" s="33">
-        <v>45034</v>
+        <v>45037</v>
       </c>
       <c r="G47" s="35" t="s">
-        <v>439</v>
+        <v>442</v>
       </c>
       <c r="H47" s="35" t="s">
-        <v>438</v>
+        <v>441</v>
       </c>
       <c r="I47" s="24" t="s">
         <v>219</v>
@@ -6833,7 +6833,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="49" spans="1:20" ht="195.75" thickBot="1">
+    <row r="49" spans="1:20" ht="225.75" thickBot="1">
       <c r="A49" s="20">
         <v>63</v>
       </c>
@@ -6873,7 +6873,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="50" spans="1:20" ht="195.75" thickBot="1">
+    <row r="50" spans="1:20" ht="225.75" thickBot="1">
       <c r="A50" s="20">
         <v>64</v>
       </c>
@@ -6913,7 +6913,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="51" spans="1:20" ht="195.75" thickBot="1">
+    <row r="51" spans="1:20" ht="225.75" thickBot="1">
       <c r="A51" s="20">
         <v>65</v>
       </c>
@@ -6967,7 +6967,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="52" spans="1:20" ht="195.75" thickBot="1">
+    <row r="52" spans="1:20" ht="225.75" thickBot="1">
       <c r="A52" s="20">
         <v>66</v>
       </c>
@@ -7021,7 +7021,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="53" spans="1:20" ht="195.75" thickBot="1">
+    <row r="53" spans="1:20" ht="225.75" thickBot="1">
       <c r="A53" s="20">
         <v>67</v>
       </c>
@@ -7075,7 +7075,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="54" spans="1:20" ht="195.75" thickBot="1">
+    <row r="54" spans="1:20" ht="240.75" thickBot="1">
       <c r="A54" s="20">
         <v>68</v>
       </c>
@@ -7114,7 +7114,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:20" ht="195.75" thickBot="1">
+    <row r="55" spans="1:20" ht="225.75" thickBot="1">
       <c r="A55" s="20">
         <v>69</v>
       </c>
@@ -7168,7 +7168,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="56" spans="1:20" ht="195.75" thickBot="1">
+    <row r="56" spans="1:20" ht="225.75" thickBot="1">
       <c r="A56" s="20">
         <v>70</v>
       </c>
@@ -7222,7 +7222,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:20" ht="195.75" thickBot="1">
+    <row r="57" spans="1:20" ht="225.75" thickBot="1">
       <c r="A57" s="20">
         <v>71</v>
       </c>
@@ -7276,7 +7276,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="58" spans="1:20" ht="195.75" thickBot="1">
+    <row r="58" spans="1:20" ht="225.75" thickBot="1">
       <c r="A58" s="20">
         <v>72</v>
       </c>
@@ -7330,7 +7330,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:20" ht="195.75" thickBot="1">
+    <row r="59" spans="1:20" ht="240.75" thickBot="1">
       <c r="A59" s="20">
         <v>73</v>
       </c>
@@ -7384,7 +7384,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="60" spans="1:20" ht="195.75" thickBot="1">
+    <row r="60" spans="1:20" ht="240.75" thickBot="1">
       <c r="A60" s="20">
         <v>74</v>
       </c>
@@ -7438,7 +7438,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="61" spans="1:20" ht="225.75" thickBot="1">
+    <row r="61" spans="1:20" ht="240.75" thickBot="1">
       <c r="A61" s="20">
         <v>32</v>
       </c>
@@ -7492,7 +7492,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="62" spans="1:20" ht="210.75" thickBot="1">
+    <row r="62" spans="1:20" ht="255.75" thickBot="1">
       <c r="A62" s="20">
         <v>40</v>
       </c>
@@ -7603,13 +7603,13 @@
         <v>45034</v>
       </c>
       <c r="G64" s="35" t="s">
-        <v>440</v>
+        <v>435</v>
       </c>
       <c r="H64" s="35" t="s">
-        <v>441</v>
+        <v>436</v>
       </c>
       <c r="I64" s="35" t="s">
-        <v>442</v>
+        <v>437</v>
       </c>
       <c r="J64" s="25" t="s">
         <v>68</v>
@@ -7654,7 +7654,7 @@
         <v>317</v>
       </c>
       <c r="F65" s="33">
-        <v>45034</v>
+        <v>45037</v>
       </c>
       <c r="G65" s="35" t="s">
         <v>445</v>
@@ -7708,7 +7708,7 @@
         <v>319</v>
       </c>
       <c r="F66" s="33">
-        <v>45034</v>
+        <v>45037</v>
       </c>
       <c r="G66" s="35" t="s">
         <v>448</v>
@@ -7762,16 +7762,16 @@
         <v>321</v>
       </c>
       <c r="F67" s="33">
-        <v>45034</v>
+        <v>45037</v>
       </c>
       <c r="G67" s="35" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="H67" s="35" t="s">
         <v>449</v>
       </c>
       <c r="I67" s="35" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="J67" s="25" t="s">
         <v>68</v>
@@ -7839,7 +7839,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="69" spans="1:20" ht="210.75" thickBot="1">
+    <row r="69" spans="1:20" ht="225.75" thickBot="1">
       <c r="A69" s="20">
         <v>152</v>
       </c>
@@ -7879,7 +7879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="70" spans="1:20" ht="210.75" thickBot="1">
+    <row r="70" spans="1:20" ht="225.75" thickBot="1">
       <c r="A70" s="20">
         <v>153</v>
       </c>
@@ -7933,7 +7933,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="71" spans="1:20" ht="210.75" thickBot="1">
+    <row r="71" spans="1:20" ht="225.75" thickBot="1">
       <c r="A71" s="20">
         <v>154</v>
       </c>
@@ -7987,7 +7987,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="72" spans="1:20" ht="210.75" thickBot="1">
+    <row r="72" spans="1:20" ht="225.75" thickBot="1">
       <c r="A72" s="20">
         <v>155</v>
       </c>
@@ -8041,7 +8041,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="73" spans="1:20" ht="210.75" thickBot="1">
+    <row r="73" spans="1:20" ht="240.75" thickBot="1">
       <c r="A73" s="20">
         <v>156</v>
       </c>
@@ -8081,7 +8081,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="74" spans="1:20" ht="210.75" thickBot="1">
+    <row r="74" spans="1:20" ht="240.75" thickBot="1">
       <c r="A74" s="20">
         <v>157</v>
       </c>
@@ -8135,7 +8135,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="75" spans="1:20" ht="210.75" thickBot="1">
+    <row r="75" spans="1:20" ht="225.75" thickBot="1">
       <c r="A75" s="20">
         <v>158</v>
       </c>
@@ -8189,7 +8189,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="76" spans="1:20" ht="195.75" thickBot="1">
+    <row r="76" spans="1:20" ht="210.75" thickBot="1">
       <c r="A76" s="20">
         <v>159</v>
       </c>
@@ -8243,7 +8243,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="77" spans="1:20" ht="195.75" thickBot="1">
+    <row r="77" spans="1:20" ht="210.75" thickBot="1">
       <c r="A77" s="20">
         <v>160</v>
       </c>
@@ -8297,7 +8297,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="78" spans="1:20" ht="210.75" thickBot="1">
+    <row r="78" spans="1:20" ht="225.75" thickBot="1">
       <c r="A78" s="20">
         <v>161</v>
       </c>
@@ -8337,7 +8337,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="79" spans="1:20" ht="210.75" thickBot="1">
+    <row r="79" spans="1:20" ht="225.75" thickBot="1">
       <c r="A79" s="20">
         <v>162</v>
       </c>
@@ -8391,7 +8391,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="80" spans="1:20" ht="210.75" thickBot="1">
+    <row r="80" spans="1:20" ht="225.75" thickBot="1">
       <c r="A80" s="20">
         <v>163</v>
       </c>
@@ -8445,7 +8445,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="81" spans="1:20" ht="210.75" thickBot="1">
+    <row r="81" spans="1:20" ht="225.75" thickBot="1">
       <c r="A81" s="20">
         <v>164</v>
       </c>
@@ -8499,7 +8499,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="82" spans="1:20" ht="210.75" thickBot="1">
+    <row r="82" spans="1:20" ht="225.75" thickBot="1">
       <c r="A82" s="20">
         <v>165</v>
       </c>
@@ -8553,7 +8553,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="83" spans="1:20" ht="210.75" thickBot="1">
+    <row r="83" spans="1:20" ht="225.75" thickBot="1">
       <c r="A83" s="20">
         <v>166</v>
       </c>
@@ -8607,7 +8607,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="84" spans="1:20" ht="210.75" thickBot="1">
+    <row r="84" spans="1:20" ht="225.75" thickBot="1">
       <c r="A84" s="20">
         <v>167</v>
       </c>
@@ -8661,7 +8661,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="85" spans="1:20" ht="210.75" thickBot="1">
+    <row r="85" spans="1:20" ht="240.75" thickBot="1">
       <c r="A85" s="20">
         <v>168</v>
       </c>
@@ -8715,7 +8715,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="86" spans="1:20" ht="210">
+    <row r="86" spans="1:20" ht="225">
       <c r="A86" s="20">
         <v>169</v>
       </c>

</xml_diff>

<commit_message>
sistemazioni segnalazioni 28 aprile 2023
</commit_message>
<xml_diff>
--- a/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
+++ b/GATEWAY/S1#111DEDALUS0000/DEDALUS_SPA/HERO/5.2/report-checklist.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Devel\GIT\it-fse-accreditamento\GATEWAY\S1#111DEDALUS0000\DEDALUS_SPA\HERO\5.2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA593D5-5686-4766-B26F-412A8AB4F88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CAD20E-081A-4E46-8140-55074D410494}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1050" yWindow="-120" windowWidth="23070" windowHeight="13740" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1692,22 +1692,22 @@
     <t>2023-04-21T18:33:10Z</t>
   </si>
   <si>
-    <t>98ce35bbd4f47cdf</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.330734ed8ddfaee1745e7cbb033f2e0ae3001fbbc75497e5e4efb1f797aa19dc.e21627db4b^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-21T18:40:58Z</t>
-  </si>
-  <si>
-    <t>21c775a9ff02c75a</t>
-  </si>
-  <si>
-    <t>2.16.840.1.113883.2.9.2.150.4.4.934167a59c9f6667655d91d04807f0b8b2283f57358e23960660542ea9ba4327.671eee0e02^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
-  </si>
-  <si>
-    <t>2023-04-21T18:55:13Z</t>
+    <t>b91b3be1db81f3a9</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.330734ed8ddfaee1745e7cbb033f2e0ae3001fbbc75497e5e4efb1f797aa19dc.63c3bd9b9f^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-28T15:47:17Z</t>
+  </si>
+  <si>
+    <t>b5a83b79395e8651</t>
+  </si>
+  <si>
+    <t>2.16.840.1.113883.2.9.2.150.4.4.934167a59c9f6667655d91d04807f0b8b2283f57358e23960660542ea9ba4327.a817f0ef73^^^^urn:ihe:iti:xdw:2013:workflowInstanceId</t>
+  </si>
+  <si>
+    <t>2023-04-28T15:55:55Z</t>
   </si>
 </sst>
 </file>
@@ -7708,7 +7708,7 @@
         <v>319</v>
       </c>
       <c r="F66" s="33">
-        <v>45037</v>
+        <v>45044</v>
       </c>
       <c r="G66" s="35" t="s">
         <v>448</v>
@@ -7762,7 +7762,7 @@
         <v>321</v>
       </c>
       <c r="F67" s="33">
-        <v>45037</v>
+        <v>45044</v>
       </c>
       <c r="G67" s="35" t="s">
         <v>451</v>

</xml_diff>